<commit_message>
+ fix + skeleton of fast product function
</commit_message>
<xml_diff>
--- a/lab1/Table1_2.xlsx
+++ b/lab1/Table1_2.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Redmi\Documents\ParallelnieVichisleniya\lab1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9FEFD72E-B0EF-41F1-BCEE-076C61C72CE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CF868EB-B410-4F90-B544-D50C64CBDF7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1920" yWindow="600" windowWidth="14616" windowHeight="12360"/>
+    <workbookView xWindow="1920" yWindow="600" windowWidth="14616" windowHeight="12360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Table1_2" sheetId="1" r:id="rId1"/>
@@ -67,7 +67,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -403,7 +403,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="23">
     <border>
       <left/>
       <right/>
@@ -529,6 +529,184 @@
         <color indexed="64"/>
       </top>
       <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -578,9 +756,21 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% — акцент1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -935,11 +1125,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+    <sheetView tabSelected="1" zoomScale="108" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -951,108 +1141,108 @@
     <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B2" s="12">
         <v>1</v>
       </c>
-      <c r="C2" s="1">
+      <c r="C2" s="12">
         <v>11.9672</v>
       </c>
-      <c r="D2" s="1">
+      <c r="D2" s="12">
         <v>18.160599999999999</v>
       </c>
-      <c r="E2" s="1">
+      <c r="E2" s="12">
         <v>31.551500000000001</v>
       </c>
-      <c r="F2" s="1">
+      <c r="F2" s="13">
         <v>38.856999999999999</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
+    <row r="3" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="1">
+      <c r="B3" s="12">
         <v>1</v>
       </c>
-      <c r="C3" s="1">
+      <c r="C3" s="12">
         <v>0.92400000000000004</v>
       </c>
-      <c r="D3" s="1">
+      <c r="D3" s="12">
         <v>1.4418</v>
       </c>
-      <c r="E3" s="1">
+      <c r="E3" s="12">
         <v>2.2332000000000001</v>
       </c>
-      <c r="F3" s="1">
+      <c r="F3" s="13">
         <v>5.3189000000000002</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
+    <row r="4" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="1">
+      <c r="B4" s="12">
         <v>1</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C4" s="12">
         <v>1.3271999999999999</v>
       </c>
-      <c r="D4" s="1">
+      <c r="D4" s="12">
         <v>1.6411</v>
       </c>
-      <c r="E4" s="1">
+      <c r="E4" s="12">
         <v>2.2852000000000001</v>
       </c>
-      <c r="F4" s="1">
+      <c r="F4" s="13">
         <v>3.3832</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="1">
+      <c r="B5" s="4">
         <v>2</v>
       </c>
-      <c r="C5" s="1">
+      <c r="C5" s="4">
         <v>0.48060000000000003</v>
       </c>
-      <c r="D5" s="1">
+      <c r="D5" s="4">
         <v>0.76170000000000004</v>
       </c>
-      <c r="E5" s="1">
+      <c r="E5" s="4">
         <v>1.6323000000000001</v>
       </c>
-      <c r="F5" s="1">
+      <c r="F5" s="5">
         <v>2.0104000000000002</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6" s="1"/>
+      <c r="A6" s="6"/>
       <c r="B6" s="1">
         <v>3</v>
       </c>
@@ -1065,50 +1255,50 @@
       <c r="E6" s="1">
         <v>1.1389</v>
       </c>
-      <c r="F6" s="1">
+      <c r="F6" s="7">
         <v>1.4438</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A7" s="1"/>
-      <c r="B7" s="1">
+    <row r="7" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="8"/>
+      <c r="B7" s="9">
         <v>4</v>
       </c>
-      <c r="C7" s="1">
+      <c r="C7" s="9">
         <v>0.2792</v>
       </c>
-      <c r="D7" s="1">
+      <c r="D7" s="9">
         <v>0.52070000000000005</v>
       </c>
-      <c r="E7" s="1">
+      <c r="E7" s="9">
         <v>0.8125</v>
       </c>
-      <c r="F7" s="1">
+      <c r="F7" s="10">
         <v>1.1688000000000001</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A8" s="1" t="s">
+      <c r="A8" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="1">
+      <c r="B8" s="4">
         <v>2</v>
       </c>
-      <c r="C8" s="1">
+      <c r="C8" s="4">
         <v>18.101299999999998</v>
       </c>
-      <c r="D8" s="1">
+      <c r="D8" s="4">
         <v>29.5259</v>
       </c>
-      <c r="E8" s="1">
+      <c r="E8" s="4">
         <v>38.702500000000001</v>
       </c>
-      <c r="F8" s="1">
+      <c r="F8" s="5">
         <v>47.960700000000003</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A9" s="1"/>
+      <c r="A9" s="6"/>
       <c r="B9" s="1">
         <v>3</v>
       </c>
@@ -1121,50 +1311,50 @@
       <c r="E9" s="1">
         <v>59.194699999999997</v>
       </c>
-      <c r="F9" s="1">
+      <c r="F9" s="7">
         <v>96.957599999999999</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1">
+    <row r="10" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="8"/>
+      <c r="B10" s="9">
         <v>4</v>
       </c>
-      <c r="C10" s="1">
+      <c r="C10" s="9">
         <v>24.777000000000001</v>
       </c>
-      <c r="D10" s="1">
+      <c r="D10" s="9">
         <v>65.276899999999998</v>
       </c>
-      <c r="E10" s="1">
+      <c r="E10" s="9">
         <v>95.870199999999997</v>
       </c>
-      <c r="F10" s="1">
+      <c r="F10" s="10">
         <v>134.05109999999999</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A11" s="1" t="s">
+      <c r="A11" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="1">
+      <c r="B11" s="4">
         <v>2</v>
       </c>
-      <c r="C11" s="1">
+      <c r="C11" s="4">
         <v>0.50490000000000002</v>
       </c>
-      <c r="D11" s="1">
+      <c r="D11" s="4">
         <v>1.9333</v>
       </c>
-      <c r="E11" s="1">
+      <c r="E11" s="4">
         <v>1.4935</v>
       </c>
-      <c r="F11" s="1">
+      <c r="F11" s="5">
         <v>2.1675</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A12" s="1"/>
+      <c r="A12" s="6"/>
       <c r="B12" s="1">
         <v>3</v>
       </c>
@@ -1177,50 +1367,50 @@
       <c r="E12" s="1">
         <v>1.8683000000000001</v>
       </c>
-      <c r="F12" s="1">
+      <c r="F12" s="7">
         <v>2.6642000000000001</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A13" s="1"/>
-      <c r="B13" s="1">
+    <row r="13" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="8"/>
+      <c r="B13" s="9">
         <v>4</v>
       </c>
-      <c r="C13" s="1">
+      <c r="C13" s="9">
         <v>0.1618</v>
       </c>
-      <c r="D13" s="1">
+      <c r="D13" s="9">
         <v>0.86050000000000004</v>
       </c>
-      <c r="E13" s="1">
+      <c r="E13" s="9">
         <v>1.9274</v>
       </c>
-      <c r="F13" s="1">
+      <c r="F13" s="10">
         <v>2.2423999999999999</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A14" s="1" t="s">
+      <c r="A14" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B14" s="1">
+      <c r="B14" s="4">
         <v>2</v>
       </c>
-      <c r="C14" s="1">
+      <c r="C14" s="4">
         <v>0.95079999999999998</v>
       </c>
-      <c r="D14" s="1">
+      <c r="D14" s="4">
         <v>1.5678000000000001</v>
       </c>
-      <c r="E14" s="1">
+      <c r="E14" s="4">
         <v>2.3940999999999999</v>
       </c>
-      <c r="F14" s="1">
+      <c r="F14" s="5">
         <v>3.6154000000000002</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A15" s="1"/>
+      <c r="A15" s="6"/>
       <c r="B15" s="1">
         <v>3</v>
       </c>
@@ -1233,50 +1423,50 @@
       <c r="E15" s="1">
         <v>2.5363000000000002</v>
       </c>
-      <c r="F15" s="1">
+      <c r="F15" s="7">
         <v>3.0044</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A16" s="1"/>
-      <c r="B16" s="1">
+    <row r="16" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="8"/>
+      <c r="B16" s="9">
         <v>4</v>
       </c>
-      <c r="C16" s="1">
+      <c r="C16" s="9">
         <v>0.59340000000000004</v>
       </c>
-      <c r="D16" s="1">
+      <c r="D16" s="9">
         <v>4.4310999999999998</v>
       </c>
-      <c r="E16" s="1">
+      <c r="E16" s="9">
         <v>3.6848999999999998</v>
       </c>
-      <c r="F16" s="1">
+      <c r="F16" s="10">
         <v>3.7040000000000002</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A17" s="1" t="s">
+      <c r="A17" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B17" s="1">
+      <c r="B17" s="4">
         <v>2</v>
       </c>
-      <c r="C17" s="1">
+      <c r="C17" s="4">
         <v>6.3078000000000003</v>
       </c>
-      <c r="D17" s="1">
+      <c r="D17" s="4">
         <v>10.361499999999999</v>
       </c>
-      <c r="E17" s="1">
+      <c r="E17" s="4">
         <v>14.496</v>
       </c>
-      <c r="F17" s="1">
+      <c r="F17" s="5">
         <v>21.1477</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A18" s="1"/>
+      <c r="A18" s="6"/>
       <c r="B18" s="1">
         <v>3</v>
       </c>
@@ -1289,30 +1479,126 @@
       <c r="E18" s="1">
         <v>9.4011999999999993</v>
       </c>
-      <c r="F18" s="1">
+      <c r="F18" s="7">
         <v>13.542</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A19" s="1"/>
-      <c r="B19" s="1">
+    <row r="19" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="8"/>
+      <c r="B19" s="9">
         <v>4</v>
       </c>
-      <c r="C19" s="1">
+      <c r="C19" s="9">
         <v>3.0581999999999998</v>
       </c>
-      <c r="D19" s="1">
+      <c r="D19" s="9">
         <v>5.6593999999999998</v>
       </c>
-      <c r="E19" s="1">
+      <c r="E19" s="9">
         <v>18.933199999999999</v>
       </c>
-      <c r="F19" s="1">
+      <c r="F19" s="10">
         <v>14.365500000000001</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="C2:F19">
+    <cfRule type="colorScale" priority="9">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C2:F2">
+    <cfRule type="colorScale" priority="8">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C3:F3">
+    <cfRule type="colorScale" priority="7">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C4:F4">
+    <cfRule type="colorScale" priority="6">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C5:F7">
+    <cfRule type="colorScale" priority="5">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C8:F10">
+    <cfRule type="colorScale" priority="4">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C11:F13">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C14:F16">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C17:F19">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>